<commit_message>
Swapped sprints 4 & 5.
</commit_message>
<xml_diff>
--- a/Documentation/Roadmap.xlsx
+++ b/Documentation/Roadmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pipin\Documents\fyp\SophieCOMP3000\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{037869EF-EE6F-433A-94F4-1E8BF1BC6B05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549D98D4-7636-4CD7-88C2-AA242277B647}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{53864A50-9EE7-4BD2-AA97-B8AECD3C4F84}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="85">
   <si>
     <t>Week 1</t>
   </si>
@@ -198,9 +198,6 @@
     <t>Stand up meeting 4</t>
   </si>
   <si>
-    <t>User story: I wish to view</t>
-  </si>
-  <si>
     <t>User story: I wish to interact with the algorithm</t>
   </si>
   <si>
@@ -210,9 +207,6 @@
     <t>Testing</t>
   </si>
   <si>
-    <t>Fixes</t>
-  </si>
-  <si>
     <t>Feedback &amp; changes</t>
   </si>
   <si>
@@ -285,10 +279,13 @@
     <t>Try without crossover and remove all parents.</t>
   </si>
   <si>
-    <t>molecule, info &amp; PES</t>
-  </si>
-  <si>
     <t>Move from test area to application.</t>
+  </si>
+  <si>
+    <t>User story: I wish to view molecule, info &amp; PES</t>
+  </si>
+  <si>
+    <t>Fixes &amp; improvements</t>
   </si>
 </sst>
 </file>
@@ -513,7 +510,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -648,9 +645,6 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -689,6 +683,16 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -698,8 +702,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF00FF00"/>
       <color rgb="FF00FFFF"/>
-      <color rgb="FF00FF00"/>
       <color rgb="FFFF3399"/>
       <color rgb="FF9966FF"/>
       <color rgb="FFFF6699"/>
@@ -1017,8 +1021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D91ADE50-0E0F-41B8-9D4D-224F0CCF1AAD}">
   <dimension ref="A1:R81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1161,7 +1165,7 @@
       <c r="M4" s="61"/>
       <c r="N4" s="62"/>
       <c r="O4" s="60" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="P4" s="61"/>
       <c r="Q4" s="63"/>
@@ -1184,12 +1188,12 @@
       <c r="J5" s="49"/>
       <c r="K5" s="52"/>
       <c r="L5" s="52" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="M5" s="52"/>
       <c r="N5" s="52"/>
       <c r="O5" s="52" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="P5" s="52"/>
       <c r="Q5" s="55"/>
@@ -1209,7 +1213,7 @@
       <c r="I6" s="49"/>
       <c r="J6" s="49"/>
       <c r="K6" s="52" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L6" s="52"/>
       <c r="M6" s="52"/>
@@ -1236,16 +1240,16 @@
       <c r="J7" s="49"/>
       <c r="K7" s="58"/>
       <c r="L7" s="58" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M7" s="58"/>
       <c r="N7" s="58"/>
       <c r="O7" s="58" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="P7" s="58"/>
-      <c r="Q7" s="78"/>
-      <c r="R7" s="78"/>
+      <c r="Q7" s="77"/>
+      <c r="R7" s="77"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" s="6"/>
@@ -1259,17 +1263,17 @@
       <c r="I8" s="49"/>
       <c r="J8" s="49"/>
       <c r="K8" s="58" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L8" s="58"/>
       <c r="M8" s="58"/>
       <c r="N8" s="58"/>
       <c r="O8" s="58" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="P8" s="58"/>
-      <c r="Q8" s="78"/>
-      <c r="R8" s="78"/>
+      <c r="Q8" s="77"/>
+      <c r="R8" s="77"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" s="7"/>
@@ -1278,24 +1282,24 @@
       <c r="D9" s="49"/>
       <c r="E9" s="49"/>
       <c r="F9" s="49"/>
-      <c r="G9" s="79"/>
-      <c r="H9" s="79" t="s">
-        <v>65</v>
-      </c>
-      <c r="I9" s="79"/>
-      <c r="J9" s="79"/>
-      <c r="K9" s="79"/>
-      <c r="L9" s="79" t="s">
-        <v>70</v>
-      </c>
-      <c r="M9" s="79"/>
-      <c r="N9" s="79"/>
-      <c r="O9" s="79"/>
-      <c r="P9" s="79" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q9" s="81"/>
-      <c r="R9" s="81"/>
+      <c r="G9" s="78"/>
+      <c r="H9" s="78" t="s">
+        <v>63</v>
+      </c>
+      <c r="I9" s="78"/>
+      <c r="J9" s="78"/>
+      <c r="K9" s="78"/>
+      <c r="L9" s="78" t="s">
+        <v>68</v>
+      </c>
+      <c r="M9" s="78"/>
+      <c r="N9" s="78"/>
+      <c r="O9" s="78"/>
+      <c r="P9" s="78" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q9" s="80"/>
+      <c r="R9" s="80"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
@@ -1306,24 +1310,24 @@
       <c r="D10" s="49"/>
       <c r="E10" s="49"/>
       <c r="F10" s="49"/>
-      <c r="G10" s="79"/>
-      <c r="H10" s="79" t="s">
-        <v>66</v>
-      </c>
-      <c r="I10" s="79"/>
-      <c r="J10" s="79"/>
-      <c r="K10" s="79"/>
-      <c r="L10" s="79" t="s">
-        <v>72</v>
-      </c>
-      <c r="M10" s="79"/>
-      <c r="N10" s="79"/>
-      <c r="O10" s="79" t="s">
-        <v>83</v>
-      </c>
-      <c r="P10" s="79"/>
-      <c r="Q10" s="81"/>
-      <c r="R10" s="81"/>
+      <c r="G10" s="78"/>
+      <c r="H10" s="78" t="s">
+        <v>64</v>
+      </c>
+      <c r="I10" s="78"/>
+      <c r="J10" s="78"/>
+      <c r="K10" s="78"/>
+      <c r="L10" s="78" t="s">
+        <v>70</v>
+      </c>
+      <c r="M10" s="78"/>
+      <c r="N10" s="78"/>
+      <c r="O10" s="78" t="s">
+        <v>81</v>
+      </c>
+      <c r="P10" s="78"/>
+      <c r="Q10" s="80"/>
+      <c r="R10" s="80"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" s="7"/>
@@ -1332,24 +1336,24 @@
       <c r="D11" s="49"/>
       <c r="E11" s="49"/>
       <c r="F11" s="49"/>
-      <c r="G11" s="79"/>
-      <c r="H11" s="79" t="s">
-        <v>67</v>
-      </c>
-      <c r="I11" s="79"/>
-      <c r="J11" s="79"/>
-      <c r="K11" s="79"/>
-      <c r="L11" s="79" t="s">
-        <v>73</v>
-      </c>
-      <c r="M11" s="79"/>
-      <c r="N11" s="79"/>
-      <c r="O11" s="79" t="s">
-        <v>85</v>
-      </c>
-      <c r="P11" s="79"/>
-      <c r="Q11" s="81"/>
-      <c r="R11" s="81"/>
+      <c r="G11" s="78"/>
+      <c r="H11" s="78" t="s">
+        <v>65</v>
+      </c>
+      <c r="I11" s="78"/>
+      <c r="J11" s="78"/>
+      <c r="K11" s="78"/>
+      <c r="L11" s="78" t="s">
+        <v>71</v>
+      </c>
+      <c r="M11" s="78"/>
+      <c r="N11" s="78"/>
+      <c r="O11" s="78" t="s">
+        <v>82</v>
+      </c>
+      <c r="P11" s="78"/>
+      <c r="Q11" s="80"/>
+      <c r="R11" s="80"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" s="7"/>
@@ -1358,18 +1362,18 @@
       <c r="D12" s="49"/>
       <c r="E12" s="49"/>
       <c r="F12" s="49"/>
-      <c r="G12" s="79"/>
-      <c r="H12" s="79" t="s">
-        <v>68</v>
-      </c>
-      <c r="I12" s="79"/>
-      <c r="J12" s="79"/>
-      <c r="K12" s="79"/>
-      <c r="L12" s="79" t="s">
-        <v>74</v>
-      </c>
-      <c r="M12" s="79"/>
-      <c r="N12" s="79"/>
+      <c r="G12" s="78"/>
+      <c r="H12" s="78" t="s">
+        <v>66</v>
+      </c>
+      <c r="I12" s="78"/>
+      <c r="J12" s="78"/>
+      <c r="K12" s="78"/>
+      <c r="L12" s="78" t="s">
+        <v>72</v>
+      </c>
+      <c r="M12" s="78"/>
+      <c r="N12" s="78"/>
       <c r="O12" s="49"/>
       <c r="P12" s="49"/>
       <c r="Q12" s="33"/>
@@ -1382,12 +1386,12 @@
       <c r="D13" s="48"/>
       <c r="E13" s="48"/>
       <c r="F13" s="48"/>
-      <c r="G13" s="80"/>
-      <c r="H13" s="80" t="s">
-        <v>69</v>
-      </c>
-      <c r="I13" s="80"/>
-      <c r="J13" s="80"/>
+      <c r="G13" s="79"/>
+      <c r="H13" s="79" t="s">
+        <v>67</v>
+      </c>
+      <c r="I13" s="79"/>
+      <c r="J13" s="79"/>
       <c r="K13" s="48"/>
       <c r="L13" s="48"/>
       <c r="M13" s="48"/>
@@ -1474,10 +1478,10 @@
       <c r="H17" s="40">
         <v>44183</v>
       </c>
-      <c r="I17" s="70" t="s">
+      <c r="I17" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="J17" s="71"/>
+      <c r="J17" s="70"/>
       <c r="K17" s="37" t="s">
         <v>11</v>
       </c>
@@ -1517,10 +1521,10 @@
       <c r="H18" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="I18" s="72" t="s">
+      <c r="I18" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="J18" s="73"/>
+      <c r="J18" s="72"/>
       <c r="K18" s="46" t="s">
         <v>40</v>
       </c>
@@ -1546,10 +1550,10 @@
       <c r="F19" s="48"/>
       <c r="G19" s="48"/>
       <c r="H19" s="48"/>
-      <c r="I19" s="72" t="s">
+      <c r="I19" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="J19" s="73"/>
+      <c r="J19" s="72"/>
       <c r="K19" s="48"/>
       <c r="L19" s="48"/>
       <c r="M19" s="48"/>
@@ -1558,26 +1562,26 @@
     <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="5"/>
       <c r="B20" s="16"/>
-      <c r="C20" s="51"/>
-      <c r="D20" s="61" t="s">
-        <v>58</v>
-      </c>
+      <c r="C20" s="52" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" s="51"/>
       <c r="E20" s="61"/>
       <c r="F20" s="62"/>
-      <c r="G20" s="52" t="s">
-        <v>55</v>
+      <c r="G20" s="61" t="s">
+        <v>57</v>
       </c>
       <c r="H20" s="52"/>
-      <c r="I20" s="72" t="s">
+      <c r="I20" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="J20" s="73"/>
-      <c r="K20" s="52" t="s">
-        <v>55</v>
+      <c r="J20" s="72"/>
+      <c r="K20" s="61" t="s">
+        <v>57</v>
       </c>
       <c r="L20" s="62"/>
       <c r="M20" s="52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N20" s="52"/>
       <c r="O20" s="51"/>
@@ -1589,21 +1593,19 @@
       </c>
       <c r="B21" s="16"/>
       <c r="C21" s="52"/>
-      <c r="D21" s="52" t="s">
-        <v>60</v>
-      </c>
+      <c r="D21" s="52"/>
       <c r="E21" s="52"/>
       <c r="F21" s="62"/>
       <c r="G21" s="52" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="H21" s="52"/>
-      <c r="I21" s="72" t="s">
+      <c r="I21" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="J21" s="73"/>
+      <c r="J21" s="72"/>
       <c r="K21" s="52" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="L21" s="62"/>
       <c r="M21" s="49"/>
@@ -1613,19 +1615,21 @@
       <c r="A22" s="5"/>
       <c r="B22" s="16"/>
       <c r="C22" s="52"/>
-      <c r="D22" s="52" t="s">
-        <v>59</v>
-      </c>
+      <c r="D22" s="51"/>
       <c r="E22" s="52"/>
       <c r="F22" s="62"/>
-      <c r="G22" s="49"/>
-      <c r="H22" s="49"/>
-      <c r="I22" s="72" t="s">
+      <c r="G22" s="52" t="s">
+        <v>84</v>
+      </c>
+      <c r="H22" s="52"/>
+      <c r="I22" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="J22" s="73"/>
-      <c r="K22" s="49"/>
-      <c r="L22" s="49"/>
+      <c r="J22" s="72"/>
+      <c r="K22" s="52" t="s">
+        <v>84</v>
+      </c>
+      <c r="L22" s="52"/>
       <c r="M22" s="49"/>
       <c r="N22" s="49"/>
     </row>
@@ -1634,20 +1638,22 @@
         <v>15</v>
       </c>
       <c r="B23" s="17"/>
-      <c r="C23" s="68"/>
-      <c r="D23" s="69" t="s">
+      <c r="C23" s="81"/>
+      <c r="D23" s="82"/>
+      <c r="E23" s="83"/>
+      <c r="F23" s="84"/>
+      <c r="G23" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="E23" s="69"/>
-      <c r="F23" s="59"/>
-      <c r="G23" s="49"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="72" t="s">
+      <c r="H23" s="58"/>
+      <c r="I23" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="J23" s="73"/>
-      <c r="K23" s="49"/>
-      <c r="L23" s="49"/>
+      <c r="J23" s="72"/>
+      <c r="K23" s="68" t="s">
+        <v>18</v>
+      </c>
+      <c r="L23" s="58"/>
       <c r="M23" s="49"/>
       <c r="N23" s="49"/>
     </row>
@@ -1660,10 +1666,10 @@
       <c r="F24" s="49"/>
       <c r="G24" s="49"/>
       <c r="H24" s="49"/>
-      <c r="I24" s="72" t="s">
+      <c r="I24" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="J24" s="73"/>
+      <c r="J24" s="72"/>
       <c r="K24" s="49"/>
       <c r="L24" s="49"/>
       <c r="M24" s="49"/>
@@ -1678,10 +1684,10 @@
       <c r="F25" s="49"/>
       <c r="G25" s="49"/>
       <c r="H25" s="49"/>
-      <c r="I25" s="72" t="s">
+      <c r="I25" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="J25" s="73"/>
+      <c r="J25" s="72"/>
       <c r="K25" s="49"/>
       <c r="L25" s="49"/>
       <c r="M25" s="49"/>
@@ -1698,10 +1704,10 @@
       <c r="F26" s="49"/>
       <c r="G26" s="49"/>
       <c r="H26" s="49"/>
-      <c r="I26" s="72" t="s">
+      <c r="I26" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="J26" s="73"/>
+      <c r="J26" s="72"/>
       <c r="K26" s="49"/>
       <c r="L26" s="49"/>
       <c r="M26" s="49"/>
@@ -1716,10 +1722,10 @@
       <c r="F27" s="49"/>
       <c r="G27" s="49"/>
       <c r="H27" s="49"/>
-      <c r="I27" s="72" t="s">
+      <c r="I27" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="J27" s="73"/>
+      <c r="J27" s="72"/>
       <c r="K27" s="49"/>
       <c r="L27" s="49"/>
       <c r="M27" s="49"/>
@@ -1734,10 +1740,10 @@
       <c r="F28" s="49"/>
       <c r="G28" s="49"/>
       <c r="H28" s="49"/>
-      <c r="I28" s="72" t="s">
+      <c r="I28" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="J28" s="73"/>
+      <c r="J28" s="72"/>
       <c r="K28" s="49"/>
       <c r="L28" s="49"/>
       <c r="M28" s="49"/>
@@ -1752,10 +1758,10 @@
       <c r="F29" s="48"/>
       <c r="G29" s="48"/>
       <c r="H29" s="48"/>
-      <c r="I29" s="74" t="s">
+      <c r="I29" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="J29" s="75"/>
+      <c r="J29" s="74"/>
       <c r="K29" s="32"/>
       <c r="L29" s="32"/>
       <c r="M29" s="32"/>
@@ -1892,7 +1898,7 @@
       <c r="F35" s="32"/>
       <c r="K35" s="32"/>
       <c r="M35" s="65" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="N35" s="66"/>
       <c r="O35" s="32"/>
@@ -1903,19 +1909,19 @@
       <c r="B36" s="16"/>
       <c r="C36" s="13"/>
       <c r="D36" s="61" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E36" s="63"/>
       <c r="F36" s="63"/>
       <c r="G36" s="13"/>
       <c r="H36" s="61" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I36" s="61"/>
       <c r="J36" s="62"/>
       <c r="K36" s="55"/>
       <c r="L36" s="55" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M36" s="55"/>
       <c r="N36" s="57"/>
@@ -1933,7 +1939,7 @@
       <c r="F37" s="33"/>
       <c r="G37" s="60"/>
       <c r="H37" s="52" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I37" s="52"/>
       <c r="J37" s="62"/>
@@ -1953,7 +1959,7 @@
       <c r="F38" s="33"/>
       <c r="G38" s="60"/>
       <c r="H38" s="52" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I38" s="52"/>
       <c r="J38" s="62"/>
@@ -1973,12 +1979,12 @@
       <c r="D39" s="33"/>
       <c r="E39" s="33"/>
       <c r="F39" s="33"/>
-      <c r="G39" s="78"/>
-      <c r="H39" s="78" t="s">
+      <c r="G39" s="77"/>
+      <c r="H39" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="I39" s="78"/>
-      <c r="J39" s="78"/>
+      <c r="I39" s="77"/>
+      <c r="J39" s="77"/>
       <c r="K39" s="33"/>
       <c r="L39" s="33"/>
       <c r="M39" s="33"/>
@@ -2163,10 +2169,10 @@
       <c r="F49" s="45">
         <v>44281</v>
       </c>
-      <c r="G49" s="70" t="s">
+      <c r="G49" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="H49" s="71"/>
+      <c r="H49" s="70"/>
       <c r="I49" s="42" t="s">
         <v>27</v>
       </c>
@@ -2201,10 +2207,10 @@
       <c r="D50" s="48"/>
       <c r="E50" s="48"/>
       <c r="F50" s="48"/>
-      <c r="G50" s="72" t="s">
+      <c r="G50" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="H50" s="76"/>
+      <c r="H50" s="75"/>
       <c r="I50" s="48"/>
       <c r="J50" s="48"/>
       <c r="K50" s="48"/>
@@ -2222,10 +2228,10 @@
       <c r="D51" s="48"/>
       <c r="E51" s="48"/>
       <c r="F51" s="48"/>
-      <c r="G51" s="72" t="s">
+      <c r="G51" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="H51" s="76"/>
+      <c r="H51" s="75"/>
       <c r="I51" s="48"/>
       <c r="J51" s="48"/>
       <c r="K51" s="48"/>
@@ -2233,7 +2239,7 @@
       <c r="M51" s="48"/>
       <c r="N51" s="48"/>
       <c r="O51" s="65" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="P51" s="67"/>
       <c r="Q51" s="64"/>
@@ -2245,10 +2251,10 @@
       <c r="D52" s="49"/>
       <c r="E52" s="49"/>
       <c r="F52" s="49"/>
-      <c r="G52" s="72" t="s">
+      <c r="G52" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="H52" s="76"/>
+      <c r="H52" s="75"/>
       <c r="I52" s="49"/>
       <c r="J52" s="49"/>
       <c r="K52" s="49"/>
@@ -2268,10 +2274,10 @@
       <c r="D53" s="49"/>
       <c r="E53" s="49"/>
       <c r="F53" s="49"/>
-      <c r="G53" s="72" t="s">
+      <c r="G53" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="H53" s="76"/>
+      <c r="H53" s="75"/>
       <c r="I53" s="49"/>
       <c r="J53" s="49"/>
       <c r="K53" s="49"/>
@@ -2289,10 +2295,10 @@
       <c r="D54" s="49"/>
       <c r="E54" s="49"/>
       <c r="F54" s="49"/>
-      <c r="G54" s="72" t="s">
+      <c r="G54" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="H54" s="76"/>
+      <c r="H54" s="75"/>
       <c r="I54" s="49"/>
       <c r="J54" s="49"/>
       <c r="K54" s="49"/>
@@ -2312,10 +2318,10 @@
       <c r="D55" s="49"/>
       <c r="E55" s="49"/>
       <c r="F55" s="49"/>
-      <c r="G55" s="72" t="s">
+      <c r="G55" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="H55" s="76"/>
+      <c r="H55" s="75"/>
       <c r="I55" s="49"/>
       <c r="J55" s="49"/>
       <c r="K55" s="49"/>
@@ -2333,10 +2339,10 @@
       <c r="D56" s="49"/>
       <c r="E56" s="49"/>
       <c r="F56" s="49"/>
-      <c r="G56" s="72" t="s">
+      <c r="G56" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="H56" s="76"/>
+      <c r="H56" s="75"/>
       <c r="I56" s="49"/>
       <c r="J56" s="49"/>
       <c r="K56" s="49"/>
@@ -2354,10 +2360,10 @@
       <c r="D57" s="49"/>
       <c r="E57" s="49"/>
       <c r="F57" s="49"/>
-      <c r="G57" s="72" t="s">
+      <c r="G57" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="H57" s="76"/>
+      <c r="H57" s="75"/>
       <c r="I57" s="49"/>
       <c r="J57" s="49"/>
       <c r="K57" s="49"/>
@@ -2377,10 +2383,10 @@
       <c r="D58" s="49"/>
       <c r="E58" s="49"/>
       <c r="F58" s="49"/>
-      <c r="G58" s="72" t="s">
+      <c r="G58" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="H58" s="76"/>
+      <c r="H58" s="75"/>
       <c r="I58" s="49"/>
       <c r="J58" s="49"/>
       <c r="K58" s="49"/>
@@ -2398,10 +2404,10 @@
       <c r="D59" s="49"/>
       <c r="E59" s="49"/>
       <c r="F59" s="49"/>
-      <c r="G59" s="72" t="s">
+      <c r="G59" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="H59" s="76"/>
+      <c r="H59" s="75"/>
       <c r="I59" s="49"/>
       <c r="J59" s="49"/>
       <c r="K59" s="49"/>
@@ -2419,10 +2425,10 @@
       <c r="D60" s="49"/>
       <c r="E60" s="49"/>
       <c r="F60" s="49"/>
-      <c r="G60" s="72" t="s">
+      <c r="G60" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="H60" s="76"/>
+      <c r="H60" s="75"/>
       <c r="I60" s="49"/>
       <c r="J60" s="49"/>
       <c r="K60" s="49"/>
@@ -2440,10 +2446,10 @@
       <c r="D61" s="48"/>
       <c r="E61" s="48"/>
       <c r="F61" s="48"/>
-      <c r="G61" s="74" t="s">
+      <c r="G61" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="H61" s="77"/>
+      <c r="H61" s="76"/>
       <c r="I61" s="48"/>
       <c r="J61" s="48"/>
       <c r="K61" s="48"/>

</xml_diff>

<commit_message>
Added plot limit info.
</commit_message>
<xml_diff>
--- a/Documentation/Roadmap.xlsx
+++ b/Documentation/Roadmap.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pipin\Documents\fyp\SophieCOMP3000\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549D98D4-7636-4CD7-88C2-AA242277B647}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E82ED7-A6A4-4C0A-A2ED-09ED6231D718}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{53864A50-9EE7-4BD2-AA97-B8AECD3C4F84}"/>
   </bookViews>

</xml_diff>

<commit_message>
Made options for the user to choose the optimisation algorithm.
</commit_message>
<xml_diff>
--- a/Documentation/Roadmap.xlsx
+++ b/Documentation/Roadmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pipin\Documents\fyp\SophieCOMP3000\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E82ED7-A6A4-4C0A-A2ED-09ED6231D718}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00377250-8EDC-469C-9A6A-D9BCBECE5AEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{53864A50-9EE7-4BD2-AA97-B8AECD3C4F84}"/>
   </bookViews>
@@ -1022,7 +1022,7 @@
   <dimension ref="A1:R81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Acted on user feedback to make interaction energy minima clearer.
</commit_message>
<xml_diff>
--- a/Documentation/Roadmap.xlsx
+++ b/Documentation/Roadmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pipin\Documents\fyp\SophieCOMP3000\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00377250-8EDC-469C-9A6A-D9BCBECE5AEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17614006-F1B6-41ED-BD03-2759A9C7CA1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{53864A50-9EE7-4BD2-AA97-B8AECD3C4F84}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="86">
   <si>
     <t>Week 1</t>
   </si>
@@ -201,18 +201,12 @@
     <t>User story: I wish to interact with the algorithm</t>
   </si>
   <si>
-    <t>User story: I wish to find isomers</t>
-  </si>
-  <si>
     <t>Testing</t>
   </si>
   <si>
     <t>Feedback &amp; changes</t>
   </si>
   <si>
-    <t>Fixes &amp; clean up</t>
-  </si>
-  <si>
     <t>Showcase materials</t>
   </si>
   <si>
@@ -286,13 +280,22 @@
   </si>
   <si>
     <t>Fixes &amp; improvements</t>
+  </si>
+  <si>
+    <t>Final fixes &amp; clean up</t>
+  </si>
+  <si>
+    <t>Finish code</t>
+  </si>
+  <si>
+    <t>Start writing report</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -360,6 +363,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -510,7 +520,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -694,6 +704,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1021,8 +1032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D91ADE50-0E0F-41B8-9D4D-224F0CCF1AAD}">
   <dimension ref="A1:R81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1165,7 +1176,7 @@
       <c r="M4" s="61"/>
       <c r="N4" s="62"/>
       <c r="O4" s="60" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P4" s="61"/>
       <c r="Q4" s="63"/>
@@ -1188,12 +1199,12 @@
       <c r="J5" s="49"/>
       <c r="K5" s="52"/>
       <c r="L5" s="52" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M5" s="52"/>
       <c r="N5" s="52"/>
       <c r="O5" s="52" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="P5" s="52"/>
       <c r="Q5" s="55"/>
@@ -1213,7 +1224,7 @@
       <c r="I6" s="49"/>
       <c r="J6" s="49"/>
       <c r="K6" s="52" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="L6" s="52"/>
       <c r="M6" s="52"/>
@@ -1240,12 +1251,12 @@
       <c r="J7" s="49"/>
       <c r="K7" s="58"/>
       <c r="L7" s="58" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="M7" s="58"/>
       <c r="N7" s="58"/>
       <c r="O7" s="58" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="P7" s="58"/>
       <c r="Q7" s="77"/>
@@ -1263,13 +1274,13 @@
       <c r="I8" s="49"/>
       <c r="J8" s="49"/>
       <c r="K8" s="58" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="L8" s="58"/>
       <c r="M8" s="58"/>
       <c r="N8" s="58"/>
       <c r="O8" s="58" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="P8" s="58"/>
       <c r="Q8" s="77"/>
@@ -1284,19 +1295,19 @@
       <c r="F9" s="49"/>
       <c r="G9" s="78"/>
       <c r="H9" s="78" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I9" s="78"/>
       <c r="J9" s="78"/>
       <c r="K9" s="78"/>
       <c r="L9" s="78" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="M9" s="78"/>
       <c r="N9" s="78"/>
       <c r="O9" s="78"/>
       <c r="P9" s="78" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q9" s="80"/>
       <c r="R9" s="80"/>
@@ -1312,18 +1323,18 @@
       <c r="F10" s="49"/>
       <c r="G10" s="78"/>
       <c r="H10" s="78" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I10" s="78"/>
       <c r="J10" s="78"/>
       <c r="K10" s="78"/>
       <c r="L10" s="78" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M10" s="78"/>
       <c r="N10" s="78"/>
       <c r="O10" s="78" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="P10" s="78"/>
       <c r="Q10" s="80"/>
@@ -1338,18 +1349,18 @@
       <c r="F11" s="49"/>
       <c r="G11" s="78"/>
       <c r="H11" s="78" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I11" s="78"/>
       <c r="J11" s="78"/>
       <c r="K11" s="78"/>
       <c r="L11" s="78" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="M11" s="78"/>
       <c r="N11" s="78"/>
       <c r="O11" s="78" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="P11" s="78"/>
       <c r="Q11" s="80"/>
@@ -1364,13 +1375,13 @@
       <c r="F12" s="49"/>
       <c r="G12" s="78"/>
       <c r="H12" s="78" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I12" s="78"/>
       <c r="J12" s="78"/>
       <c r="K12" s="78"/>
       <c r="L12" s="78" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="M12" s="78"/>
       <c r="N12" s="78"/>
@@ -1388,7 +1399,7 @@
       <c r="F13" s="48"/>
       <c r="G13" s="79"/>
       <c r="H13" s="79" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I13" s="79"/>
       <c r="J13" s="79"/>
@@ -1563,13 +1574,13 @@
       <c r="A20" s="5"/>
       <c r="B20" s="16"/>
       <c r="C20" s="52" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D20" s="51"/>
       <c r="E20" s="61"/>
       <c r="F20" s="62"/>
       <c r="G20" s="61" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H20" s="52"/>
       <c r="I20" s="71" t="s">
@@ -1577,7 +1588,7 @@
       </c>
       <c r="J20" s="72"/>
       <c r="K20" s="61" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L20" s="62"/>
       <c r="M20" s="52" t="s">
@@ -1597,7 +1608,7 @@
       <c r="E21" s="52"/>
       <c r="F21" s="62"/>
       <c r="G21" s="52" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H21" s="52"/>
       <c r="I21" s="71" t="s">
@@ -1605,7 +1616,7 @@
       </c>
       <c r="J21" s="72"/>
       <c r="K21" s="52" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L21" s="62"/>
       <c r="M21" s="49"/>
@@ -1619,7 +1630,7 @@
       <c r="E22" s="52"/>
       <c r="F22" s="62"/>
       <c r="G22" s="52" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H22" s="52"/>
       <c r="I22" s="71" t="s">
@@ -1627,7 +1638,7 @@
       </c>
       <c r="J22" s="72"/>
       <c r="K22" s="52" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="L22" s="52"/>
       <c r="M22" s="49"/>
@@ -1896,9 +1907,13 @@
       <c r="D35" s="32"/>
       <c r="E35" s="32"/>
       <c r="F35" s="32"/>
+      <c r="I35" s="85" t="s">
+        <v>84</v>
+      </c>
+      <c r="J35" s="85"/>
       <c r="K35" s="32"/>
       <c r="M35" s="65" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="N35" s="66"/>
       <c r="O35" s="32"/>
@@ -1911,17 +1926,17 @@
       <c r="D36" s="61" t="s">
         <v>56</v>
       </c>
-      <c r="E36" s="63"/>
-      <c r="F36" s="63"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="61" t="s">
-        <v>57</v>
-      </c>
-      <c r="I36" s="61"/>
-      <c r="J36" s="62"/>
+      <c r="E36" s="61"/>
+      <c r="F36" s="62"/>
+      <c r="G36" s="51"/>
+      <c r="H36" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="I36" s="51"/>
+      <c r="J36" s="51"/>
       <c r="K36" s="55"/>
       <c r="L36" s="55" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="M36" s="55"/>
       <c r="N36" s="57"/>
@@ -1933,16 +1948,18 @@
         <v>14</v>
       </c>
       <c r="B37" s="16"/>
-      <c r="C37" s="33"/>
-      <c r="D37" s="33"/>
-      <c r="E37" s="33"/>
-      <c r="F37" s="33"/>
-      <c r="G37" s="60"/>
-      <c r="H37" s="52" t="s">
-        <v>58</v>
-      </c>
-      <c r="I37" s="52"/>
-      <c r="J37" s="62"/>
+      <c r="C37" s="60"/>
+      <c r="D37" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="E37" s="52"/>
+      <c r="F37" s="62"/>
+      <c r="G37" s="51"/>
+      <c r="H37" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="I37" s="51"/>
+      <c r="J37" s="51"/>
       <c r="K37" s="33"/>
       <c r="L37" s="33"/>
       <c r="M37" s="33"/>
@@ -1953,16 +1970,10 @@
     <row r="38" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A38" s="5"/>
       <c r="B38" s="16"/>
-      <c r="C38" s="33"/>
-      <c r="D38" s="33"/>
-      <c r="E38" s="33"/>
-      <c r="F38" s="33"/>
-      <c r="G38" s="60"/>
-      <c r="H38" s="52" t="s">
-        <v>59</v>
-      </c>
-      <c r="I38" s="52"/>
-      <c r="J38" s="62"/>
+      <c r="C38" s="60"/>
+      <c r="D38" s="52"/>
+      <c r="E38" s="52"/>
+      <c r="F38" s="62"/>
       <c r="K38" s="33"/>
       <c r="L38" s="33"/>
       <c r="M38" s="33"/>
@@ -1975,16 +1986,12 @@
         <v>15</v>
       </c>
       <c r="B39" s="17"/>
-      <c r="C39" s="33"/>
-      <c r="D39" s="33"/>
-      <c r="E39" s="33"/>
-      <c r="F39" s="33"/>
-      <c r="G39" s="77"/>
-      <c r="H39" s="77" t="s">
+      <c r="C39" s="77"/>
+      <c r="D39" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="I39" s="77"/>
-      <c r="J39" s="77"/>
+      <c r="E39" s="77"/>
+      <c r="F39" s="77"/>
       <c r="K39" s="33"/>
       <c r="L39" s="33"/>
       <c r="M39" s="33"/>
@@ -2239,7 +2246,7 @@
       <c r="M51" s="48"/>
       <c r="N51" s="48"/>
       <c r="O51" s="65" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="P51" s="67"/>
       <c r="Q51" s="64"/>

</xml_diff>